<commit_message>
Add fault into simulink model
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/NET_NYPS_68Bus/NETS_NYPS_68Bus.xlsx
+++ b/Examples/AcPowerSystem/NET_NYPS_68Bus/NETS_NYPS_68Bus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\NET_NYPS_68Bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224BFD7A-B268-40F4-9666-7E40F93F9CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFA4AA0-358F-482C-9D9B-7837BB22E5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -3292,7 +3292,7 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3340,8 +3340,8 @@
         <v>300</v>
       </c>
       <c r="D3" s="14">
-        <f>0.25*C3/10</f>
-        <v>7.5</v>
+        <f>0.25*C3</f>
+        <v>75</v>
       </c>
       <c r="E3" s="14">
         <v>4.1000000000000003E-3</v>
@@ -3362,8 +3362,8 @@
         <v>30.2</v>
       </c>
       <c r="D4" s="14">
-        <f t="shared" ref="D4:D18" si="0">0.25*C4/10</f>
-        <v>0.755</v>
+        <f>0.25*C4</f>
+        <v>7.55</v>
       </c>
       <c r="E4" s="14">
         <v>3.5000000000000003E-2</v>
@@ -3385,8 +3385,8 @@
         <v>35.799999999999997</v>
       </c>
       <c r="D5" s="14">
-        <f t="shared" si="0"/>
-        <v>0.89499999999999991</v>
+        <f>0.25*C5</f>
+        <v>8.9499999999999993</v>
       </c>
       <c r="E5" s="14">
         <v>3.04E-2</v>
@@ -3407,8 +3407,8 @@
         <v>28.6</v>
       </c>
       <c r="D6" s="14">
-        <f t="shared" si="0"/>
-        <v>0.71500000000000008</v>
+        <f t="shared" ref="D6:D18" si="0">0.25*C6</f>
+        <v>7.15</v>
       </c>
       <c r="E6" s="14">
         <v>2.9499999999999998E-2</v>
@@ -3430,7 +3430,7 @@
       </c>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
-        <v>0.65</v>
+        <v>6.5</v>
       </c>
       <c r="E7" s="14">
         <v>2.7E-2</v>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
-        <v>0.86999999999999988</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E8" s="14">
         <v>2.24E-2</v>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="D9" s="14">
         <f t="shared" si="0"/>
-        <v>0.65999999999999992</v>
+        <v>6.6</v>
       </c>
       <c r="E9" s="14">
         <v>3.2199999999999999E-2</v>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="D10" s="14">
         <f t="shared" si="0"/>
-        <v>0.60750000000000004</v>
+        <v>6.0750000000000002</v>
       </c>
       <c r="E10" s="14">
         <v>2.8000000000000001E-2</v>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="D11" s="14">
         <f t="shared" si="0"/>
-        <v>0.86250000000000004</v>
+        <v>8.625</v>
       </c>
       <c r="E11" s="14">
         <v>2.98E-2</v>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="D12" s="14">
         <f t="shared" si="0"/>
-        <v>0.77500000000000002</v>
+        <v>7.75</v>
       </c>
       <c r="E12" s="14">
         <v>1.9900000000000001E-2</v>
@@ -3562,7 +3562,7 @@
       </c>
       <c r="D13" s="14">
         <f t="shared" si="0"/>
-        <v>0.70499999999999996</v>
+        <v>7.05</v>
       </c>
       <c r="E13" s="14">
         <v>1.03E-2</v>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="D14" s="14">
         <f t="shared" si="0"/>
-        <v>2.3075000000000001</v>
+        <v>23.074999999999999</v>
       </c>
       <c r="E14" s="14">
         <v>2.1999999999999999E-2</v>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="D15" s="14">
         <f t="shared" si="0"/>
-        <v>6.2</v>
+        <v>62</v>
       </c>
       <c r="E15" s="14">
         <v>3.0000000000000001E-3</v>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="D16" s="14">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>75</v>
       </c>
       <c r="E16" s="14">
         <v>1.6999999999999999E-3</v>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="D17" s="14">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>75</v>
       </c>
       <c r="E17" s="14">
         <v>1.6999999999999999E-3</v>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="D18" s="14">
         <f t="shared" si="0"/>
-        <v>1.05</v>
+        <v>10.5</v>
       </c>
       <c r="E18" s="14">
         <v>1.2500000000000001E-2</v>

</xml_diff>